<commit_message>
implementar nmudar ip facil endpoint e leitura de sensores
</commit_message>
<xml_diff>
--- a/pesquisas/Pasta1.xlsx
+++ b/pesquisas/Pasta1.xlsx
@@ -24,25 +24,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>BINÁRIO</t>
-  </si>
-  <si>
-    <t>HEXADECIMAL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>CÓDIGO DTC</t>
+    <t>Valores</t>
+  </si>
+  <si>
+    <t>Hexadecimal</t>
+  </si>
+  <si>
+    <t>Binário</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código DTC </t>
+  </si>
+  <si>
+    <t>Unidade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,16 +56,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -82,17 +102,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -375,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R4"/>
+  <dimension ref="B2:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:R1"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -387,151 +475,156 @@
     <col min="3" max="18" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-    </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3">
-        <v>2</v>
-      </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3">
-        <v>3</v>
-      </c>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2">
         <v>0</v>
       </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
+      <c r="F3" s="2"/>
       <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
       <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>1</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
       <c r="O3" s="2">
-        <v>0</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>1</v>
-      </c>
-      <c r="R3" s="2">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3">
-        <v>1</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3">
+      <c r="C5" s="4">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="4">
         <v>2</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3">
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="4">
         <v>3</v>
       </c>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="K1:R1"/>
+  <mergeCells count="10">
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="C2:R2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>